<commit_message>
Change Class: => ERef in Type-column
</commit_message>
<xml_diff>
--- a/EquipmentModelBulkLoadTool/WaterPumpSystem.xlsx
+++ b/EquipmentModelBulkLoadTool/WaterPumpSystem.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Examples\EquipmentModelBulkLoadTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\example\EquipmentModelBulkLoadTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FBFDCE-3B9D-4F57-870A-05F3C18672AF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214EA31-F42E-4F4C-A629-9673834EC3FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{D10EB2D3-CC97-4C6D-951D-ECF021B19BCF}"/>
+    <workbookView xWindow="13800" yWindow="2250" windowWidth="24345" windowHeight="17760" xr2:uid="{D10EB2D3-CC97-4C6D-951D-ECF021B19BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t>Source tank</t>
   </si>
   <si>
-    <t>Class:Tank</t>
-  </si>
-  <si>
     <t>The tank, from which the pump is pumping</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
     <t>Instance: Tank</t>
   </si>
   <si>
+    <t>Parent</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
@@ -240,7 +240,7 @@
     <t>Flowback pipe</t>
   </si>
   <si>
-    <t>Parent</t>
+    <t>ERef:Tank</t>
   </si>
 </sst>
 </file>
@@ -694,24 +694,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0402A82-1F84-44B1-B6D0-67B8091469A0}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="41" customWidth="1"/>
-    <col min="3" max="3" width="52" customWidth="1"/>
-    <col min="4" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" customWidth="1"/>
-    <col min="7" max="7" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -728,7 +728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -742,7 +742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -759,7 +759,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -770,7 +770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -781,7 +781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -795,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -809,7 +809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -823,58 +823,58 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
-        <v>33</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>1</v>
@@ -883,20 +883,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>1</v>
@@ -908,39 +908,39 @@
         <v>3</v>
       </c>
       <c r="E39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>37</v>
-      </c>
-      <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
         <v>39</v>
-      </c>
-      <c r="D40" t="s">
-        <v>40</v>
       </c>
       <c r="E40" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
       </c>
       <c r="C41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" t="s">
         <v>42</v>
-      </c>
-      <c r="D41" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -954,30 +954,30 @@
   <dimension ref="A7:K16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" customWidth="1"/>
-    <col min="5" max="5" width="18.54296875" customWidth="1"/>
-    <col min="6" max="6" width="21.1796875" customWidth="1"/>
-    <col min="7" max="7" width="33.453125" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="10" width="28.81640625" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" customWidth="1"/>
-    <col min="12" max="12" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>68</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>45</v>
@@ -986,10 +986,10 @@
         <v>46</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>47</v>
@@ -1007,7 +1007,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>52</v>
       </c>
@@ -1036,12 +1036,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -1059,22 +1059,22 @@
         <v>22222</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F11" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
     </row>
   </sheetData>
@@ -1094,28 +1094,28 @@
   <dimension ref="A4:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>62</v>
@@ -1124,7 +1124,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1134,31 +1134,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{754FE1FE-0F6A-43FD-834A-BA19EF346159}">
   <dimension ref="A7:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.54296875" customWidth="1"/>
-    <col min="2" max="2" width="39.54296875" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" customWidth="1"/>
-    <col min="5" max="5" width="23.81640625" customWidth="1"/>
-    <col min="6" max="6" width="40.1796875" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" customWidth="1"/>
-    <col min="11" max="11" width="19.1796875" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>45</v>
@@ -1176,7 +1176,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>65</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
update syntax to refer others equipment property
</commit_message>
<xml_diff>
--- a/EquipmentModelBulkLoadTool/WaterPumpSystem.xlsx
+++ b/EquipmentModelBulkLoadTool/WaterPumpSystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\example\EquipmentModelBulkLoadTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Examples\EquipmentModelBulkLoadTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3214EA31-F42E-4F4C-A629-9673834EC3FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CBF703-AB2F-43E3-B623-A924B537B3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="2250" windowWidth="24345" windowHeight="17760" xr2:uid="{D10EB2D3-CC97-4C6D-951D-ECF021B19BCF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D10EB2D3-CC97-4C6D-951D-ECF021B19BCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Types" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Class : Pipe : Mechanical device</t>
   </si>
@@ -240,7 +240,10 @@
     <t>Flowback pipe</t>
   </si>
   <si>
-    <t>ERef:Tank</t>
+    <t>ReferenceTarget</t>
+  </si>
+  <si>
+    <t>Class:Path_Tank</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1"/>
@@ -376,6 +379,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -695,7 +700,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -781,7 +786,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -794,8 +799,11 @@
       <c r="D19" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -808,8 +816,9 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -822,30 +831,31 @@
       <c r="D21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
       <c r="C22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>68</v>
-      </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -855,8 +865,9 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -866,13 +877,14 @@
       <c r="C25" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="13"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>